<commit_message>
All Exceptions are handled and status is also updating accordingly
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -606,7 +606,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" activeCellId="1" sqref="B16 B7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>